<commit_message>
Registro: Crear encabezados principales
Crear el nombre de los encabezados principales del archivo para
crear la base de datos en el registro.

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_ventas.xlsx
+++ b/registro_ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467F04E-FEAF-41D3-8601-A6A3BB2A7181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7629A6-C8A6-45A5-8E99-61FBCE81EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
+    <workbookView xWindow="1725" yWindow="1725" windowWidth="12000" windowHeight="7845" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,50 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>CANT</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>TALLA</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>TIPO DE PAGO</t>
+  </si>
+  <si>
+    <t>A CUENTA</t>
+  </si>
+  <si>
+    <t>EFECTIVO</t>
+  </si>
+  <si>
+    <t>TARJETA</t>
+  </si>
+  <si>
+    <t>TOTAL DE VENTA</t>
+  </si>
+  <si>
+    <t>CIERRE/DIA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +425,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E54BC-2388-4289-9894-A5CEAA9ACA7E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Registro: Crear formato como tabla
Crear formato como tabla para el registro

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_ventas.xlsx
+++ b/registro_ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7629A6-C8A6-45A5-8E99-61FBCE81EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D926F4A-813D-44FE-8154-874D46014B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="1725" windowWidth="12000" windowHeight="7845" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>FECHA</t>
   </si>
@@ -96,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -104,13 +104,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,57 +492,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E54BC-2388-4289-9894-A5CEAA9ACA7E}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Registro: Establecer formato a toda la tabla
* Agregar formato a toda la tabla.
* Cambia el tipo de letra.
* Agregar color de letra para columnas específicas.
* Agregar fórmulas de suma a la tabla de datos contables.
* Establecer tamaño predeterminado de celdas.
* Configurar la fila TOTAL para la contabilidad del registro.

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_ventas.xlsx
+++ b/registro_ventas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D926F4A-813D-44FE-8154-874D46014B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA93739-CAAC-4829-9EA8-A633220D822F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
+    <workbookView xWindow="1725" yWindow="1725" windowWidth="12000" windowHeight="7845" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,16 +90,80 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -126,60 +193,125 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,391 +624,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E54BC-2388-4289-9894-A5CEAA9ACA7E}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-    </row>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="20"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+      <c r="B24" s="22" t="str">
+        <f>SUM(B4:B23)&amp;" Artículos"</f>
+        <v>0 Artículos</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="12">
+        <f>SUM(I4:I23)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="12">
+        <f>SUM(J4:J23)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <f>SUM(I24:J24)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <f>SUM(K4:K23)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <f>SUM(L24)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Registro: Mostrar el día de la semana con respecto a la fecha
* Muestra el día de la semana con respecto a la fecha usando la funcion TEXTO

  =TEXTO(valor, texto_con_formato)

* Usar MAYUSC para mostrarlo en mayúsculas.

  =MAYUSC(TEXTO(valor, "texto_con_formato"))

Signed_off_by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_ventas.xlsx
+++ b/registro_ventas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA93739-CAAC-4829-9EA8-A633220D822F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E6D74B-688D-4B88-9A05-646D11A45E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="1725" windowWidth="12000" windowHeight="7845" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
@@ -82,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +142,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2E1500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -243,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,12 +288,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -307,6 +307,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -627,7 +634,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,12 +655,17 @@
     <col min="14" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="str">
+        <f>UPPER(TEXT(A4,"DDDD"))</f>
+        <v>SÁBADO</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -694,302 +706,302 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="19"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="20"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="19"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="20"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="19"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="19"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="19"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="19"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="19"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="19"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="19"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="19"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="19"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="19"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="19"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="19"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="19"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="19"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="19"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="19"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="19"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="20"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="19"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="19"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="20"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="19"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="19"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="20"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="19"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="19"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
@@ -997,7 +1009,7 @@
       <c r="A24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="22" t="str">
+      <c r="B24" s="20" t="str">
         <f>SUM(B4:B23)&amp;" Artículos"</f>
         <v>0 Artículos</v>
       </c>

</xml_diff>

<commit_message>
Registro: Aplicar formato a la columna de fecha
* Utilizar formato "dd-mmm-aa" para devolver la fecha en texto.

Signed-off-by: qaotyk <mayniakgd@gmail.com>
</commit_message>
<xml_diff>
--- a/registro_ventas.xlsx
+++ b/registro_ventas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QAOTYK\Desktop\registro_excel_macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E6D74B-688D-4B88-9A05-646D11A45E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6789AC8F-73AB-43B9-BA52-83F1CBAD5745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="1725" windowWidth="12000" windowHeight="7845" xr2:uid="{D3AF314D-D49C-4E56-878F-BFC4E127C6E3}"/>
   </bookViews>
@@ -294,18 +294,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -314,6 +308,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,7 +634,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,16 +656,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="21"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="str">
+      <c r="A2" s="21" t="str">
         <f>UPPER(TEXT(A4,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -706,13 +706,13 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="17"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="18"/>
+      <c r="G4" s="17"/>
       <c r="H4" s="5"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -721,13 +721,13 @@
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="5"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -736,13 +736,13 @@
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="5"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -751,13 +751,13 @@
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="5"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -766,13 +766,13 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="17"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="5"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -781,13 +781,13 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="17"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="5"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -796,13 +796,13 @@
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="17"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="5"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -811,13 +811,13 @@
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="17"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="5"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -826,13 +826,13 @@
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="17"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="5"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -841,13 +841,13 @@
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="5"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -856,13 +856,13 @@
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="5"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -871,13 +871,13 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="17"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="18"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="5"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -886,13 +886,13 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="18"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="5"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -901,13 +901,13 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="17"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="17"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="5"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -916,13 +916,13 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="17"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="17"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="18"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="5"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -931,13 +931,13 @@
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="17"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="17"/>
       <c r="H19" s="5"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -946,13 +946,13 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="17"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="18"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="5"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -961,13 +961,13 @@
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="17"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="18"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="5"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -976,13 +976,13 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="18"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="5"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -991,13 +991,13 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="17"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="17"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="18"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="5"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1009,7 +1009,7 @@
       <c r="A24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="20" t="str">
+      <c r="B24" s="18" t="str">
         <f>SUM(B4:B23)&amp;" Artículos"</f>
         <v>0 Artículos</v>
       </c>

</xml_diff>